<commit_message>
setup geo scripts and added IYCF coverages to spreadsheets
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Tanzania/2017Sep/regions/InputForCode_Arusha_IYCF.xlsx
+++ b/input_spreadsheets/Tanzania/2017Sep/regions/InputForCode_Arusha_IYCF.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28209"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/Github Projects/Nutrition/input_spreadsheets/Tanzania/2017Sep/regions/IYCFonly/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20220" yWindow="-20160" windowWidth="18160" windowHeight="19280" tabRatio="500" firstSheet="17" activeTab="20"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14700" tabRatio="500" firstSheet="17" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="demographics" sheetId="1" r:id="rId1"/>
@@ -40,11 +35,11 @@
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -1324,7 +1319,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1398,6 +1393,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="61">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
@@ -2882,12 +2878,12 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="32.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2895,7 +2891,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -2903,7 +2899,7 @@
         <v>330679</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
@@ -2911,7 +2907,7 @@
         <v>53388.654589770274</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1">
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
@@ -2919,7 +2915,7 @@
         <v>62773.657901275794</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>71</v>
       </c>
@@ -2927,7 +2923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1">
       <c r="A6" s="5" t="s">
         <v>70</v>
       </c>
@@ -2935,7 +2931,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1">
       <c r="A7" s="5" t="s">
         <v>72</v>
       </c>
@@ -2947,6 +2943,11 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2959,12 +2960,12 @@
       <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="2" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
@@ -2987,7 +2988,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -3010,7 +3011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="B3" s="5" t="s">
         <v>46</v>
       </c>
@@ -3030,7 +3031,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="B4" s="5" t="s">
         <v>47</v>
       </c>
@@ -3050,7 +3051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="B5" s="5" t="s">
         <v>48</v>
       </c>
@@ -3070,7 +3071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -3093,7 +3094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="B7" s="5" t="s">
         <v>46</v>
       </c>
@@ -3113,7 +3114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="B8" s="5" t="s">
         <v>47</v>
       </c>
@@ -3133,7 +3134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="B9" s="5" t="s">
         <v>48</v>
       </c>
@@ -3153,7 +3154,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -3176,7 +3177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="B11" s="5" t="s">
         <v>46</v>
       </c>
@@ -3196,7 +3197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="B12" s="5" t="s">
         <v>47</v>
       </c>
@@ -3216,7 +3217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="B13" s="5" t="s">
         <v>48</v>
       </c>
@@ -3236,7 +3237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -3259,7 +3260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="B15" s="5" t="s">
         <v>46</v>
       </c>
@@ -3279,7 +3280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="B16" s="5" t="s">
         <v>47</v>
       </c>
@@ -3299,7 +3300,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1">
       <c r="B17" s="5" t="s">
         <v>48</v>
       </c>
@@ -3319,7 +3320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -3342,7 +3343,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1">
       <c r="B19" s="5" t="s">
         <v>46</v>
       </c>
@@ -3362,7 +3363,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1">
       <c r="B20" s="5" t="s">
         <v>47</v>
       </c>
@@ -3382,7 +3383,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1">
       <c r="B21" s="5" t="s">
         <v>48</v>
       </c>
@@ -3402,7 +3403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:7" ht="15.75" customHeight="1">
       <c r="A22" t="s">
         <v>36</v>
       </c>
@@ -3425,7 +3426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:7" ht="15.75" customHeight="1">
       <c r="B23" s="5" t="s">
         <v>46</v>
       </c>
@@ -3445,7 +3446,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:7" ht="15.75" customHeight="1">
       <c r="B24" s="5" t="s">
         <v>47</v>
       </c>
@@ -3465,7 +3466,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:7" ht="15.75" customHeight="1">
       <c r="B25" s="5" t="s">
         <v>48</v>
       </c>
@@ -3485,7 +3486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:7" ht="15.75" customHeight="1">
       <c r="A26" t="s">
         <v>37</v>
       </c>
@@ -3508,7 +3509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:7" ht="15.75" customHeight="1">
       <c r="B27" s="5" t="s">
         <v>46</v>
       </c>
@@ -3528,7 +3529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:7" ht="15.75" customHeight="1">
       <c r="B28" s="5" t="s">
         <v>47</v>
       </c>
@@ -3548,7 +3549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:7" ht="15.75" customHeight="1">
       <c r="B29" s="5" t="s">
         <v>48</v>
       </c>
@@ -3570,6 +3571,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3582,13 +3588,13 @@
       <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="33.83203125" customWidth="1"/>
     <col min="2" max="2" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
@@ -3605,7 +3611,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" s="8" t="s">
         <v>16</v>
       </c>
@@ -3624,7 +3630,7 @@
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="A3" s="8" t="s">
         <v>21</v>
       </c>
@@ -3643,7 +3649,7 @@
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="A4" s="8" t="s">
         <v>22</v>
       </c>
@@ -3662,7 +3668,7 @@
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="A5" s="8" t="s">
         <v>24</v>
       </c>
@@ -3681,7 +3687,7 @@
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" s="8" t="s">
         <v>27</v>
       </c>
@@ -3700,7 +3706,7 @@
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="A7" s="8" t="s">
         <v>28</v>
       </c>
@@ -3719,7 +3725,7 @@
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="A8" s="8" t="s">
         <v>54</v>
       </c>
@@ -3738,7 +3744,7 @@
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="A9" s="8" t="s">
         <v>31</v>
       </c>
@@ -3757,113 +3763,118 @@
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="B10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="B11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="B12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="B13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="B14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="B15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="B16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
     </row>
-    <row r="17" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:7" ht="15.75" customHeight="1">
       <c r="B17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
     </row>
-    <row r="18" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:7" ht="15.75" customHeight="1">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
     </row>
-    <row r="19" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:7" ht="15.75" customHeight="1">
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
     </row>
-    <row r="20" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:7" ht="15.75" customHeight="1">
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
     </row>
-    <row r="21" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:7" ht="15.75" customHeight="1">
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
     </row>
-    <row r="22" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:7" ht="15.75" customHeight="1">
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
     </row>
-    <row r="23" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:7" ht="15.75" customHeight="1">
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
     </row>
-    <row r="24" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="2:7" ht="15.75" customHeight="1">
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
     </row>
-    <row r="25" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="2:7" ht="15.75" customHeight="1">
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
     </row>
-    <row r="26" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="2:7" ht="15.75" customHeight="1">
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
     </row>
-    <row r="27" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="2:7" ht="15.75" customHeight="1">
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
     </row>
-    <row r="28" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="2:7" ht="15.75" customHeight="1">
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
     </row>
-    <row r="29" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="2:7" ht="15.75" customHeight="1">
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3876,9 +3887,9 @@
       <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -3892,7 +3903,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" ht="15.75" customHeight="1">
       <c r="A2" s="5">
         <v>45</v>
       </c>
@@ -3908,6 +3919,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3918,12 +3934,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="25.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>55</v>
       </c>
@@ -3943,7 +3959,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>45</v>
       </c>
@@ -3963,7 +3979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>46</v>
       </c>
@@ -3983,7 +3999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1">
       <c r="A4" s="5" t="s">
         <v>47</v>
       </c>
@@ -4003,7 +4019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>48</v>
       </c>
@@ -4025,6 +4041,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4037,9 +4058,9 @@
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>49</v>
       </c>
@@ -4059,7 +4080,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>34</v>
       </c>
@@ -4081,6 +4102,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4093,9 +4119,9 @@
       <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1">
       <c r="A1" s="9" t="s">
         <v>53</v>
       </c>
@@ -4109,7 +4135,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="15.75" customHeight="1">
       <c r="A2" s="10">
         <v>1</v>
       </c>
@@ -4125,6 +4151,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4137,12 +4168,12 @@
       <selection activeCell="E30" sqref="E29:E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="37.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>56</v>
       </c>
@@ -4162,7 +4193,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>73</v>
       </c>
@@ -4182,7 +4213,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -4190,7 +4221,7 @@
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -4198,7 +4229,7 @@
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -4209,6 +4240,11 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4219,12 +4255,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="70.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>76</v>
       </c>
@@ -4244,7 +4280,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>57</v>
       </c>
@@ -4264,7 +4300,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>58</v>
       </c>
@@ -4284,7 +4320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1">
       <c r="A4" s="5" t="s">
         <v>59</v>
       </c>
@@ -4304,7 +4340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>60</v>
       </c>
@@ -4326,6 +4362,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4336,13 +4377,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="43.1640625" customWidth="1"/>
     <col min="2" max="6" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>56</v>
       </c>
@@ -4362,7 +4403,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>79</v>
       </c>
@@ -4384,6 +4425,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4394,12 +4440,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="5" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -4416,7 +4462,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="14">
       <c r="A2" s="11" t="s">
         <v>45</v>
       </c>
@@ -4433,14 +4479,14 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
     </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -4449,6 +4495,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4461,13 +4512,13 @@
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="12.5" customWidth="1"/>
     <col min="2" max="2" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -4475,7 +4526,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1">
       <c r="A2" s="4">
         <v>2017</v>
       </c>
@@ -4483,7 +4534,7 @@
         <v>54420.276000000005</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1">
       <c r="A3" s="4">
         <v>2018</v>
       </c>
@@ -4491,7 +4542,7 @@
         <v>55451.94</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1">
       <c r="A4" s="4">
         <v>2019</v>
       </c>
@@ -4499,7 +4550,7 @@
         <v>56741.520000000004</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1">
       <c r="A5" s="4">
         <v>2020</v>
       </c>
@@ -4507,7 +4558,7 @@
         <v>57773.184000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1">
       <c r="A6" s="4">
         <v>2021</v>
       </c>
@@ -4515,7 +4566,7 @@
         <v>58804.848000000005</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1">
       <c r="A7" s="4">
         <v>2022</v>
       </c>
@@ -4523,7 +4574,7 @@
         <v>60094.428</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1">
       <c r="A8" s="4">
         <v>2023</v>
       </c>
@@ -4531,7 +4582,7 @@
         <v>61384.008000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1">
       <c r="A9" s="4">
         <v>2024</v>
       </c>
@@ -4539,7 +4590,7 @@
         <v>62415.672000000006</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1">
       <c r="A10" s="4">
         <v>2025</v>
       </c>
@@ -4547,7 +4598,7 @@
         <v>63963.168000000005</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1">
       <c r="A11" s="4">
         <v>2026</v>
       </c>
@@ -4555,7 +4606,7 @@
         <v>65252.748000000007</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:2" ht="15.75" customHeight="1">
       <c r="A12" s="4">
         <v>2027</v>
       </c>
@@ -4563,7 +4614,7 @@
         <v>66542.328000000009</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:2" ht="15.75" customHeight="1">
       <c r="A13" s="4">
         <v>2028</v>
       </c>
@@ -4571,7 +4622,7 @@
         <v>67831.90800000001</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:2" ht="15.75" customHeight="1">
       <c r="A14" s="4">
         <v>2029</v>
       </c>
@@ -4579,7 +4630,7 @@
         <v>69379.40400000001</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:2" ht="15.75" customHeight="1">
       <c r="A15" s="4">
         <v>2030</v>
       </c>
@@ -4589,6 +4640,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4597,11 +4653,11 @@
   <sheetPr codeName="Sheet20" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="37.83203125" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
@@ -4609,7 +4665,7 @@
     <col min="4" max="4" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>56</v>
       </c>
@@ -4623,7 +4679,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>64</v>
       </c>
@@ -4640,7 +4696,7 @@
       <c r="F2" s="14"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>74</v>
       </c>
@@ -4657,7 +4713,7 @@
       <c r="F3" s="14"/>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="A4" t="s">
         <v>75</v>
       </c>
@@ -4671,7 +4727,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="A5" t="s">
         <v>77</v>
       </c>
@@ -4688,7 +4744,7 @@
       <c r="F5" s="14"/>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" s="5" t="s">
         <v>78</v>
       </c>
@@ -4705,12 +4761,12 @@
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="A7" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="B7" s="19">
-        <v>0</v>
+      <c r="B7" s="39">
+        <v>0.10703370168494016</v>
       </c>
       <c r="C7" s="38">
         <v>0.95</v>
@@ -4722,72 +4778,72 @@
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="B8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="B9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="B10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
     </row>
-    <row r="17" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:3" ht="15.75" customHeight="1">
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
     </row>
-    <row r="18" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:3" ht="15.75" customHeight="1">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
     </row>
-    <row r="19" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:3" ht="15.75" customHeight="1">
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
     </row>
-    <row r="20" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:3" ht="15.75" customHeight="1">
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
     </row>
-    <row r="21" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:3" ht="15.75" customHeight="1">
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
     </row>
-    <row r="22" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:3" ht="15.75" customHeight="1">
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
     </row>
@@ -4795,6 +4851,11 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4803,11 +4864,11 @@
   <sheetPr codeName="Sheet21" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="37.6640625" customWidth="1"/>
     <col min="2" max="6" width="13.5" customWidth="1"/>
@@ -4817,7 +4878,7 @@
     <col min="10" max="10" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>56</v>
       </c>
@@ -4842,7 +4903,7 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>64</v>
       </c>
@@ -4865,7 +4926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:10" ht="15.75" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>74</v>
       </c>
@@ -4890,7 +4951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:10" ht="15.75" customHeight="1">
       <c r="A4" t="s">
         <v>75</v>
       </c>
@@ -4914,7 +4975,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:10" ht="15.75" customHeight="1">
       <c r="A5" t="s">
         <v>77</v>
       </c>
@@ -4937,7 +4998,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:10" ht="15.75" customHeight="1">
       <c r="A6" s="5" t="s">
         <v>78</v>
       </c>
@@ -4960,7 +5021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:10" ht="15.75" customHeight="1">
       <c r="A7" s="5" t="s">
         <v>79</v>
       </c>
@@ -4983,65 +5044,65 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:10" ht="15.75" customHeight="1">
       <c r="B8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:10" ht="15.75" customHeight="1">
       <c r="B9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:10" ht="15.75" customHeight="1">
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
     </row>
-    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:10" ht="15.75" customHeight="1">
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
     </row>
-    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:10" ht="15.75" customHeight="1">
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
     </row>
-    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:10" ht="15.75" customHeight="1">
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
     </row>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:10" ht="15.75" customHeight="1">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
     </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:10" ht="15.75" customHeight="1">
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
     </row>
-    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:10" ht="15.75" customHeight="1">
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
     </row>
-    <row r="17" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:3" ht="15.75" customHeight="1">
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
     </row>
-    <row r="18" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:3" ht="15.75" customHeight="1">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
     </row>
-    <row r="19" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:3" ht="15.75" customHeight="1">
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
     </row>
-    <row r="20" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:3" ht="15.75" customHeight="1">
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
     </row>
-    <row r="21" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:3" ht="15.75" customHeight="1">
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
     </row>
@@ -5049,6 +5110,11 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5061,12 +5127,12 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="33.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>56</v>
       </c>
@@ -5086,7 +5152,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" t="s">
         <v>75</v>
       </c>
@@ -5106,7 +5172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1">
       <c r="B3" t="s">
         <v>69</v>
       </c>
@@ -5125,7 +5191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1">
       <c r="A4" t="s">
         <v>77</v>
       </c>
@@ -5145,7 +5211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1">
       <c r="B5" t="s">
         <v>69</v>
       </c>
@@ -5162,14 +5228,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1">
       <c r="A6" s="5"/>
       <c r="C6" s="18"/>
       <c r="D6" s="18"/>
       <c r="E6" s="18"/>
       <c r="F6" s="15"/>
     </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1">
       <c r="C7" s="18"/>
       <c r="D7" s="18"/>
       <c r="E7" s="18"/>
@@ -5179,6 +5245,11 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5191,12 +5262,12 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>68</v>
       </c>
@@ -5219,7 +5290,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>64</v>
       </c>
@@ -5242,7 +5313,7 @@
         <v>0.41599999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="B3" s="5" t="s">
         <v>36</v>
       </c>
@@ -5262,7 +5333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="A4" s="5" t="s">
         <v>78</v>
       </c>
@@ -5285,7 +5356,7 @@
         <v>0.41599999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="B5" s="5" t="s">
         <v>36</v>
       </c>
@@ -5309,6 +5380,11 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5321,12 +5397,12 @@
       <selection activeCell="A4" sqref="A4:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="28.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>68</v>
       </c>
@@ -5349,7 +5425,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>64</v>
       </c>
@@ -5372,7 +5448,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="B3" s="5" t="s">
         <v>36</v>
       </c>
@@ -5392,7 +5468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="A4" s="5" t="s">
         <v>78</v>
       </c>
@@ -5418,7 +5494,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="B5" s="5" t="s">
         <v>36</v>
       </c>
@@ -5442,6 +5518,11 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5454,12 +5535,12 @@
       <selection activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="28.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>68</v>
       </c>
@@ -5482,7 +5563,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>64</v>
       </c>
@@ -5505,7 +5586,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="B3" s="5" t="s">
         <v>36</v>
       </c>
@@ -5525,7 +5606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="A4" s="5" t="s">
         <v>78</v>
       </c>
@@ -5551,7 +5632,7 @@
         <v>0.496</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="B5" s="5" t="s">
         <v>36</v>
       </c>
@@ -5575,6 +5656,11 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5587,9 +5673,9 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -5600,7 +5686,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" ht="15.75" customHeight="1">
       <c r="A2" s="33">
         <v>23</v>
       </c>
@@ -5615,6 +5701,11 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5627,12 +5718,12 @@
       <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -5652,7 +5743,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -5672,7 +5763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -5692,7 +5783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -5712,7 +5803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -5732,7 +5823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -5752,7 +5843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -5772,7 +5863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:6" ht="15.75" customHeight="1">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -5792,7 +5883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:6" ht="15.75" customHeight="1">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -5812,7 +5903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:6" ht="15.75" customHeight="1">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -5832,7 +5923,7 @@
         <v>0.1368</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:6" ht="15.75" customHeight="1">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -5852,7 +5943,7 @@
         <v>0.20660000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:6" ht="15.75" customHeight="1">
       <c r="A12" t="s">
         <v>37</v>
       </c>
@@ -5872,7 +5963,7 @@
         <v>2.1100000000000001E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:6" ht="15.75" customHeight="1">
       <c r="A13" t="s">
         <v>38</v>
       </c>
@@ -5892,7 +5983,7 @@
         <v>7.4999999999999997E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:6" ht="15.75" customHeight="1">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -5912,7 +6003,7 @@
         <v>8.6199999999999999E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:6" ht="15.75" customHeight="1">
       <c r="A15" t="s">
         <v>40</v>
       </c>
@@ -5932,7 +6023,7 @@
         <v>2.86E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:6" ht="15.75" customHeight="1">
       <c r="A16" t="s">
         <v>41</v>
       </c>
@@ -5952,7 +6043,7 @@
         <v>1.5299999999999999E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:6" ht="15.75" customHeight="1">
       <c r="A17" t="s">
         <v>42</v>
       </c>
@@ -5972,7 +6063,7 @@
         <v>0.13589999999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:6" ht="15.75" customHeight="1">
       <c r="A18" t="s">
         <v>43</v>
       </c>
@@ -5999,6 +6090,11 @@
   <colBreaks count="1" manualBreakCount="1">
     <brk id="8" max="1048575" man="1"/>
   </colBreaks>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -6011,9 +6107,9 @@
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>17</v>
       </c>
@@ -6036,7 +6132,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>19</v>
       </c>
@@ -6064,7 +6160,7 @@
         <v>21.839457279977402</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="B3" s="5" t="s">
         <v>29</v>
       </c>
@@ -6089,7 +6185,7 @@
         <v>36.959379929324918</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="B4" s="5" t="s">
         <v>32</v>
       </c>
@@ -6109,7 +6205,7 @@
         <v>27.312017491552375</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="B5" s="5" t="s">
         <v>33</v>
       </c>
@@ -6129,7 +6225,7 @@
         <v>13.889145299145298</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" s="5" t="s">
         <v>35</v>
       </c>
@@ -6152,7 +6248,7 @@
         <v>48.515000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="B7" s="5" t="s">
         <v>29</v>
       </c>
@@ -6172,7 +6268,7 @@
         <v>48.515000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="B8" s="5" t="s">
         <v>32</v>
       </c>
@@ -6192,7 +6288,7 @@
         <v>2.2399999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="B9" s="5" t="s">
         <v>33</v>
       </c>
@@ -6212,7 +6308,7 @@
         <v>0.73</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" s="5" t="s">
         <v>44</v>
       </c>
@@ -6235,7 +6331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="B11" s="5" t="s">
         <v>46</v>
       </c>
@@ -6255,7 +6351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="B12" s="5" t="s">
         <v>47</v>
       </c>
@@ -6275,7 +6371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="B13" s="5" t="s">
         <v>48</v>
       </c>
@@ -6300,6 +6396,11 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -6312,9 +6413,9 @@
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>23</v>
       </c>
@@ -6325,7 +6426,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" ht="15.75" customHeight="1">
       <c r="A2" s="34">
         <v>1.9255813953488372E-2</v>
       </c>
@@ -6338,6 +6439,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -6350,9 +6456,9 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>49</v>
       </c>
@@ -6372,7 +6478,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>34</v>
       </c>
@@ -6392,7 +6498,7 @@
         <v>1.5916779661016949</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>36</v>
       </c>
@@ -6416,6 +6522,11 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -6426,9 +6537,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
@@ -6451,7 +6562,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -6474,7 +6585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="B3" s="5" t="s">
         <v>29</v>
       </c>
@@ -6494,7 +6605,7 @@
         <v>1.67</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="B4" s="5" t="s">
         <v>32</v>
       </c>
@@ -6514,7 +6625,7 @@
         <v>2.38</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="B5" s="5" t="s">
         <v>33</v>
       </c>
@@ -6534,7 +6645,7 @@
         <v>6.33</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -6557,7 +6668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="B7" s="5" t="s">
         <v>29</v>
       </c>
@@ -6577,7 +6688,7 @@
         <v>1.55</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="B8" s="5" t="s">
         <v>32</v>
       </c>
@@ -6597,7 +6708,7 @@
         <v>2.1800000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="B9" s="5" t="s">
         <v>33</v>
       </c>
@@ -6617,7 +6728,7 @@
         <v>6.39</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -6640,7 +6751,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="B11" s="5" t="s">
         <v>29</v>
       </c>
@@ -6660,7 +6771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="B12" s="5" t="s">
         <v>32</v>
       </c>
@@ -6680,7 +6791,7 @@
         <v>2.79</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="B13" s="5" t="s">
         <v>33</v>
       </c>
@@ -6700,7 +6811,7 @@
         <v>6.01</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -6723,7 +6834,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="B15" s="5" t="s">
         <v>29</v>
       </c>
@@ -6743,7 +6854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="B16" s="5" t="s">
         <v>32</v>
       </c>
@@ -6763,7 +6874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1">
       <c r="B17" s="5" t="s">
         <v>33</v>
       </c>
@@ -6783,7 +6894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1">
       <c r="A18" t="s">
         <v>43</v>
       </c>
@@ -6806,7 +6917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1">
       <c r="B19" s="5" t="s">
         <v>29</v>
       </c>
@@ -6826,7 +6937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1">
       <c r="B20" s="5" t="s">
         <v>32</v>
       </c>
@@ -6846,7 +6957,7 @@
         <v>1.86</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1">
       <c r="B21" s="5" t="s">
         <v>33</v>
       </c>
@@ -6868,6 +6979,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -6878,9 +6994,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
@@ -6903,7 +7019,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -6926,7 +7042,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="B3" s="5" t="s">
         <v>29</v>
       </c>
@@ -6946,7 +7062,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="B4" s="5" t="s">
         <v>32</v>
       </c>
@@ -6966,7 +7082,7 @@
         <v>3.41</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="B5" s="5" t="s">
         <v>33</v>
       </c>
@@ -6986,7 +7102,7 @@
         <v>12.33</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -7009,7 +7125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="B7" s="5" t="s">
         <v>29</v>
       </c>
@@ -7029,7 +7145,7 @@
         <v>1.92</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="B8" s="5" t="s">
         <v>32</v>
       </c>
@@ -7049,7 +7165,7 @@
         <v>4.66</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="B9" s="5" t="s">
         <v>33</v>
       </c>
@@ -7069,7 +7185,7 @@
         <v>9.68</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -7092,7 +7208,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="B11" s="5" t="s">
         <v>29</v>
       </c>
@@ -7112,7 +7228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="B12" s="5" t="s">
         <v>32</v>
       </c>
@@ -7132,7 +7248,7 @@
         <v>2.58</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="B13" s="5" t="s">
         <v>33</v>
       </c>
@@ -7152,7 +7268,7 @@
         <v>9.6300000000000008</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -7175,7 +7291,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="B15" s="5" t="s">
         <v>29</v>
       </c>
@@ -7195,7 +7311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="B16" s="5" t="s">
         <v>32</v>
       </c>
@@ -7215,7 +7331,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1">
       <c r="B17" s="5" t="s">
         <v>33</v>
       </c>
@@ -7235,7 +7351,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1">
       <c r="A18" t="s">
         <v>43</v>
       </c>
@@ -7258,7 +7374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1">
       <c r="B19" s="5" t="s">
         <v>29</v>
       </c>
@@ -7278,7 +7394,7 @@
         <v>1.65</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1">
       <c r="B20" s="5" t="s">
         <v>32</v>
       </c>
@@ -7298,7 +7414,7 @@
         <v>2.73</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1">
       <c r="B21" s="5" t="s">
         <v>33</v>
       </c>
@@ -7320,5 +7436,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>